<commit_message>
Best listings analysis almost done
</commit_message>
<xml_diff>
--- a/Scripts/DistrictPriceAnalysis/FlatsPriceDataPivot.xlsx
+++ b/Scripts/DistrictPriceAnalysis/FlatsPriceDataPivot.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulius\Documents\GitHub\HousingMarketAnalysis\Scripts\DistrictPriceAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E76298F-63C3-4A30-962B-64AF902A5B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237C6ECD-5905-460B-A041-D97D7E3FD35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26850" yWindow="1365" windowWidth="19410" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="38610" windowHeight="21705" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
     <sheet name="FlatsPriceDataPivot" sheetId="1" r:id="rId2"/>
+    <sheet name="SortedData" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="93">
   <si>
     <t>City</t>
   </si>
@@ -2888,7 +2889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -3040,9 +3041,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection sqref="A1:E84"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4473,6 +4479,1455 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
+    <sortCondition ref="E2:E84"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388958D7-CE0E-4A8D-9295-2E57B08647B9}">
+  <dimension ref="A1:E84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>978</v>
+      </c>
+      <c r="D2">
+        <v>7.65</v>
+      </c>
+      <c r="E2">
+        <v>127.83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1216.42</v>
+      </c>
+      <c r="D3">
+        <v>8.99</v>
+      </c>
+      <c r="E3">
+        <v>135.27000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1280.45</v>
+      </c>
+      <c r="D4">
+        <v>8.86</v>
+      </c>
+      <c r="E4">
+        <v>144.57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1096.83</v>
+      </c>
+      <c r="D5">
+        <v>7.07</v>
+      </c>
+      <c r="E5">
+        <v>155.05000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>1030.73</v>
+      </c>
+      <c r="D6">
+        <v>6.56</v>
+      </c>
+      <c r="E6">
+        <v>157.08000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>786.93</v>
+      </c>
+      <c r="D7">
+        <v>4.95</v>
+      </c>
+      <c r="E7">
+        <v>159.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>1071.45</v>
+      </c>
+      <c r="D8">
+        <v>6.58</v>
+      </c>
+      <c r="E8">
+        <v>162.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>1186.97</v>
+      </c>
+      <c r="D9">
+        <v>7.27</v>
+      </c>
+      <c r="E9">
+        <v>163.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>1702.11</v>
+      </c>
+      <c r="D10">
+        <v>10.16</v>
+      </c>
+      <c r="E10">
+        <v>167.49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>1532.1</v>
+      </c>
+      <c r="D11">
+        <v>9.06</v>
+      </c>
+      <c r="E11">
+        <v>169.17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>1865.58</v>
+      </c>
+      <c r="D12">
+        <v>10.84</v>
+      </c>
+      <c r="E12">
+        <v>172.11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>1385.18</v>
+      </c>
+      <c r="D13">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="E13">
+        <v>172.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>1544.92</v>
+      </c>
+      <c r="D14">
+        <v>8.93</v>
+      </c>
+      <c r="E14">
+        <v>173.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>1720.12</v>
+      </c>
+      <c r="D15">
+        <v>9.91</v>
+      </c>
+      <c r="E15">
+        <v>173.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>1452.92</v>
+      </c>
+      <c r="D16">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="E16">
+        <v>175.29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>1502.13</v>
+      </c>
+      <c r="D17">
+        <v>8.48</v>
+      </c>
+      <c r="E17">
+        <v>177.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>1431.24</v>
+      </c>
+      <c r="D18">
+        <v>8.07</v>
+      </c>
+      <c r="E18">
+        <v>177.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>1058.72</v>
+      </c>
+      <c r="D19">
+        <v>5.95</v>
+      </c>
+      <c r="E19">
+        <v>178.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>1396.73</v>
+      </c>
+      <c r="D20">
+        <v>7.82</v>
+      </c>
+      <c r="E20">
+        <v>178.65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>1310.01</v>
+      </c>
+      <c r="D21">
+        <v>7.33</v>
+      </c>
+      <c r="E21">
+        <v>178.72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>1724.74</v>
+      </c>
+      <c r="D22">
+        <v>9.4</v>
+      </c>
+      <c r="E22">
+        <v>183.48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>1978.65</v>
+      </c>
+      <c r="D23">
+        <v>10.78</v>
+      </c>
+      <c r="E23">
+        <v>183.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>1382.9</v>
+      </c>
+      <c r="D24">
+        <v>7.4</v>
+      </c>
+      <c r="E24">
+        <v>186.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>1826.96</v>
+      </c>
+      <c r="D25">
+        <v>9.75</v>
+      </c>
+      <c r="E25">
+        <v>187.42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>1677.92</v>
+      </c>
+      <c r="D26">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E26">
+        <v>187.58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>1123.28</v>
+      </c>
+      <c r="D27">
+        <v>5.97</v>
+      </c>
+      <c r="E27">
+        <v>188.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>1063</v>
+      </c>
+      <c r="D28">
+        <v>5.61</v>
+      </c>
+      <c r="E28">
+        <v>189.52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>1707.61</v>
+      </c>
+      <c r="D29">
+        <v>9.01</v>
+      </c>
+      <c r="E29">
+        <v>189.59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>1802.96</v>
+      </c>
+      <c r="D30">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="E30">
+        <v>190.86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31">
+        <v>1497.9</v>
+      </c>
+      <c r="D31">
+        <v>7.8</v>
+      </c>
+      <c r="E31">
+        <v>192.12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <v>1502.92</v>
+      </c>
+      <c r="D32">
+        <v>7.78</v>
+      </c>
+      <c r="E32">
+        <v>193.06</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>1928.04</v>
+      </c>
+      <c r="D33">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="E33">
+        <v>195.11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>1373.68</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>196.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>2150.7199999999998</v>
+      </c>
+      <c r="D35">
+        <v>10.82</v>
+      </c>
+      <c r="E35">
+        <v>198.86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>1175.77</v>
+      </c>
+      <c r="D36">
+        <v>5.9</v>
+      </c>
+      <c r="E36">
+        <v>199.23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>1698.9</v>
+      </c>
+      <c r="D37">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="E37">
+        <v>199.26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>1808.35</v>
+      </c>
+      <c r="D38">
+        <v>9.06</v>
+      </c>
+      <c r="E38">
+        <v>199.54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>1588.58</v>
+      </c>
+      <c r="D39">
+        <v>7.96</v>
+      </c>
+      <c r="E39">
+        <v>199.58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>1836.49</v>
+      </c>
+      <c r="D40">
+        <v>9.17</v>
+      </c>
+      <c r="E40">
+        <v>200.21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41">
+        <v>1325.7</v>
+      </c>
+      <c r="D41">
+        <v>6.59</v>
+      </c>
+      <c r="E41">
+        <v>201.28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>1027.33</v>
+      </c>
+      <c r="D42">
+        <v>5.07</v>
+      </c>
+      <c r="E42">
+        <v>202.59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43">
+        <v>1831.63</v>
+      </c>
+      <c r="D43">
+        <v>8.99</v>
+      </c>
+      <c r="E43">
+        <v>203.71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <v>2011.59</v>
+      </c>
+      <c r="D44">
+        <v>9.75</v>
+      </c>
+      <c r="E44">
+        <v>206.23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>1880.21</v>
+      </c>
+      <c r="D45">
+        <v>9.1</v>
+      </c>
+      <c r="E45">
+        <v>206.72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46">
+        <v>1147.27</v>
+      </c>
+      <c r="D46">
+        <v>5.53</v>
+      </c>
+      <c r="E46">
+        <v>207.44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47">
+        <v>1040.05</v>
+      </c>
+      <c r="D47">
+        <v>4.99</v>
+      </c>
+      <c r="E47">
+        <v>208.26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>1367.48</v>
+      </c>
+      <c r="D48">
+        <v>6.53</v>
+      </c>
+      <c r="E48">
+        <v>209.54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49">
+        <v>1421.03</v>
+      </c>
+      <c r="D49">
+        <v>6.77</v>
+      </c>
+      <c r="E49">
+        <v>209.89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50">
+        <v>1888.81</v>
+      </c>
+      <c r="D50">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E50">
+        <v>210.94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51">
+        <v>2378.1999999999998</v>
+      </c>
+      <c r="D51">
+        <v>11.21</v>
+      </c>
+      <c r="E51">
+        <v>212.12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52">
+        <v>1107.69</v>
+      </c>
+      <c r="D52">
+        <v>5.21</v>
+      </c>
+      <c r="E52">
+        <v>212.68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53">
+        <v>988.24</v>
+      </c>
+      <c r="D53">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E53">
+        <v>212.95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54">
+        <v>1671.72</v>
+      </c>
+      <c r="D54">
+        <v>7.83</v>
+      </c>
+      <c r="E54">
+        <v>213.44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55">
+        <v>2973.59</v>
+      </c>
+      <c r="D55">
+        <v>13.91</v>
+      </c>
+      <c r="E55">
+        <v>213.72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56">
+        <v>2031.25</v>
+      </c>
+      <c r="D56">
+        <v>9.5</v>
+      </c>
+      <c r="E56">
+        <v>213.91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57">
+        <v>2359.0300000000002</v>
+      </c>
+      <c r="D57">
+        <v>10.98</v>
+      </c>
+      <c r="E57">
+        <v>214.83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58">
+        <v>1328.29</v>
+      </c>
+      <c r="D58">
+        <v>6.15</v>
+      </c>
+      <c r="E58">
+        <v>215.86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59">
+        <v>3007.04</v>
+      </c>
+      <c r="D59">
+        <v>13.89</v>
+      </c>
+      <c r="E59">
+        <v>216.42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60">
+        <v>2109.71</v>
+      </c>
+      <c r="D60">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="E60">
+        <v>217.33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61">
+        <v>1640.56</v>
+      </c>
+      <c r="D61">
+        <v>7.41</v>
+      </c>
+      <c r="E61">
+        <v>221.41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62">
+        <v>2359.2600000000002</v>
+      </c>
+      <c r="D62">
+        <v>10.64</v>
+      </c>
+      <c r="E62">
+        <v>221.65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63">
+        <v>2211.41</v>
+      </c>
+      <c r="D63">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="E63">
+        <v>222.02</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64">
+        <v>2431.77</v>
+      </c>
+      <c r="D64">
+        <v>10.95</v>
+      </c>
+      <c r="E64">
+        <v>222.03</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65">
+        <v>2096.67</v>
+      </c>
+      <c r="D65">
+        <v>9.41</v>
+      </c>
+      <c r="E65">
+        <v>222.81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66">
+        <v>1050.68</v>
+      </c>
+      <c r="D66">
+        <v>4.67</v>
+      </c>
+      <c r="E66">
+        <v>225.13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67">
+        <v>2324.9</v>
+      </c>
+      <c r="D67">
+        <v>10.31</v>
+      </c>
+      <c r="E67">
+        <v>225.48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68">
+        <v>1198.07</v>
+      </c>
+      <c r="D68">
+        <v>5.31</v>
+      </c>
+      <c r="E68">
+        <v>225.61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69">
+        <v>1155.6500000000001</v>
+      </c>
+      <c r="D69">
+        <v>5.04</v>
+      </c>
+      <c r="E69">
+        <v>229.15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70">
+        <v>2589.36</v>
+      </c>
+      <c r="D70">
+        <v>11.19</v>
+      </c>
+      <c r="E70">
+        <v>231.35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71">
+        <v>1076.3</v>
+      </c>
+      <c r="D71">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E71">
+        <v>232.04</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72">
+        <v>5204.6099999999997</v>
+      </c>
+      <c r="D72">
+        <v>22.31</v>
+      </c>
+      <c r="E72">
+        <v>233.24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73">
+        <v>2015.04</v>
+      </c>
+      <c r="D73">
+        <v>8.48</v>
+      </c>
+      <c r="E73">
+        <v>237.58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74">
+        <v>3097.9</v>
+      </c>
+      <c r="D74">
+        <v>12.84</v>
+      </c>
+      <c r="E74">
+        <v>241.29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75">
+        <v>2059.38</v>
+      </c>
+      <c r="D75">
+        <v>8.4</v>
+      </c>
+      <c r="E75">
+        <v>245.19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76">
+        <v>2669.51</v>
+      </c>
+      <c r="D76">
+        <v>10.84</v>
+      </c>
+      <c r="E76">
+        <v>246.22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77">
+        <v>3911.91</v>
+      </c>
+      <c r="D77">
+        <v>15.85</v>
+      </c>
+      <c r="E77">
+        <v>246.78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78">
+        <v>2488.2600000000002</v>
+      </c>
+      <c r="D78">
+        <v>10.01</v>
+      </c>
+      <c r="E78">
+        <v>248.47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>69</v>
+      </c>
+      <c r="C79">
+        <v>3826.3</v>
+      </c>
+      <c r="D79">
+        <v>15.07</v>
+      </c>
+      <c r="E79">
+        <v>253.99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80">
+        <v>3508.93</v>
+      </c>
+      <c r="D80">
+        <v>13.54</v>
+      </c>
+      <c r="E80">
+        <v>259.13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81">
+        <v>2514.83</v>
+      </c>
+      <c r="D81">
+        <v>9.5</v>
+      </c>
+      <c r="E81">
+        <v>264.64999999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82">
+        <v>1822.18</v>
+      </c>
+      <c r="D82">
+        <v>6.56</v>
+      </c>
+      <c r="E82">
+        <v>277.94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83">
+        <v>3188.42</v>
+      </c>
+      <c r="D83">
+        <v>11.04</v>
+      </c>
+      <c r="E83">
+        <v>288.74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84">
+        <v>2016.72</v>
+      </c>
+      <c r="D84">
+        <v>5.28</v>
+      </c>
+      <c r="E84">
+        <v>381.71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Capstone analysis is done
</commit_message>
<xml_diff>
--- a/Scripts/DistrictPriceAnalysis/FlatsPriceDataPivot.xlsx
+++ b/Scripts/DistrictPriceAnalysis/FlatsPriceDataPivot.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulius\Documents\GitHub\HousingMarketAnalysis\Scripts\DistrictPriceAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237C6ECD-5905-460B-A041-D97D7E3FD35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010626C8-4815-4FB8-951E-A8E1A7659EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="38610" windowHeight="21705" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="0" windowWidth="19410" windowHeight="21705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
-    <sheet name="FlatsPriceDataPivot" sheetId="1" r:id="rId2"/>
+    <sheet name="Pivot" sheetId="3" r:id="rId1"/>
+    <sheet name="FlatsPriceData" sheetId="1" r:id="rId2"/>
     <sheet name="SortedData" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -1010,7 +1010,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$4:$A$10</c:f>
+              <c:f>Pivot!$A$4:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1039,7 +1039,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$4:$D$10</c:f>
+              <c:f>Pivot!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1888,7 +1888,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Paulius" refreshedDate="44821.713473379627" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="83" xr:uid="{00000000-000A-0000-FFFF-FFFF07000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E84" sheet="FlatsPriceDataPivot"/>
+    <worksheetSource ref="A1:E84" sheet="FlatsPriceData"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="City" numFmtId="0">
@@ -3041,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection sqref="A1:E84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4490,7 +4490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388958D7-CE0E-4A8D-9295-2E57B08647B9}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>

</xml_diff>